<commit_message>
Correciones de la entrega. Listo.
</commit_message>
<xml_diff>
--- a/documentacion/Tiempo de ejecución.xlsx
+++ b/documentacion/Tiempo de ejecución.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thyrat\Desktop\SistemasDeEcuacionesLineales\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laboratorios\Desktop\Sistemas de Ecuaciones Lineales\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -231,7 +231,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -315,6 +315,51 @@
               </a:effectLst>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-AR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Hoja1!$B$3:$B$12</c:f>
@@ -394,6 +439,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0F99-466B-92DC-D1B3BC285EA5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -477,7 +527,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -512,7 +562,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="301405728"/>
@@ -590,7 +640,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -625,7 +675,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="301406120"/>
@@ -677,7 +727,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1530,8 +1580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>